<commit_message>
first exponential trendline approximation
</commit_message>
<xml_diff>
--- a/ups runtime graph.xlsx
+++ b/ups runtime graph.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>x (watts)</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>Note: For better decimal expansion use geogebra with the following:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approximation: </t>
+  </si>
+  <si>
+    <t>y = 5279,9225284961258 * e ^ -0,0055250579809x</t>
   </si>
 </sst>
 </file>
@@ -1369,10 +1375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,19 +1481,27 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>